<commit_message>
EtherCAT Motor Control Unit EMCU documentation
</commit_message>
<xml_diff>
--- a/Robots/AR4/Axis Calculations.xlsx
+++ b/Robots/AR4/Axis Calculations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dale\Documents\GitHub\ArfBotOS\Robots\AR4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3B3CC4-66A1-4BEC-89D2-814D4557AE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAC97B3-650A-40BE-A324-6A99C769F48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15345" xr2:uid="{BC95E908-8886-4A1F-AE2F-C946640122CC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CODESYS" sheetId="2" r:id="rId1"/>
+    <sheet name="TwinCAT" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Drive Output Scale</t>
   </si>
@@ -87,6 +88,27 @@
   </si>
   <si>
     <t>Encoder</t>
+  </si>
+  <si>
+    <t>inc</t>
+  </si>
+  <si>
+    <t>motor turns</t>
+  </si>
+  <si>
+    <t>gear output turns</t>
+  </si>
+  <si>
+    <t>units in application</t>
+  </si>
+  <si>
+    <t>Increments per User Units (Deg)</t>
+  </si>
+  <si>
+    <t>Max Lag Error In User Units</t>
+  </si>
+  <si>
+    <t>Lag Error In Increments</t>
   </si>
 </sst>
 </file>
@@ -96,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000000000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +137,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -189,13 +219,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -207,6 +252,29 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -543,45 +611,393 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5CF762-EE50-4516-9624-ECA299F3B35B}">
+  <dimension ref="B3:R9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" customWidth="1"/>
+    <col min="17" max="18" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="D3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="16"/>
+      <c r="O3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(10*4)</f>
+        <v>40</v>
+      </c>
+      <c r="E4" s="13">
+        <v>400</v>
+      </c>
+      <c r="F4" s="14">
+        <f>D4*E4</f>
+        <v>16000</v>
+      </c>
+      <c r="H4" s="10">
+        <v>160000</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10">
+        <v>360</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="12">
+        <f t="shared" ref="O4:O8" si="0">(H4/I4)*(J4/K4)*(L4/M4)</f>
+        <v>444.44444444444446</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="10">
+        <v>5</v>
+      </c>
+      <c r="R4" s="12">
+        <f t="shared" ref="R4:R8" si="1">Q4*O4</f>
+        <v>2222.2222222222222</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" s="13">
+        <v>400</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" ref="F5:F9" si="2">D5*E5</f>
+        <v>20000</v>
+      </c>
+      <c r="H5" s="10">
+        <v>200000</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10">
+        <v>1</v>
+      </c>
+      <c r="M5" s="10">
+        <v>360</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="12">
+        <f t="shared" si="0"/>
+        <v>555.55555555555554</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="10">
+        <v>5</v>
+      </c>
+      <c r="R5" s="12">
+        <f t="shared" si="1"/>
+        <v>2777.7777777777778</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>50</v>
+      </c>
+      <c r="E6" s="13">
+        <v>400</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+      <c r="H6" s="10">
+        <v>200000</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10">
+        <v>1</v>
+      </c>
+      <c r="M6" s="10">
+        <v>360</v>
+      </c>
+      <c r="N6" s="7"/>
+      <c r="O6" s="12">
+        <f t="shared" si="0"/>
+        <v>555.55555555555554</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="10">
+        <v>5</v>
+      </c>
+      <c r="R6" s="12">
+        <f t="shared" si="1"/>
+        <v>2777.7777777777778</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <f>16*(28/10)</f>
+        <v>44.8</v>
+      </c>
+      <c r="E7" s="13">
+        <v>600</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="2"/>
+        <v>26880</v>
+      </c>
+      <c r="H7" s="10">
+        <v>4000</v>
+      </c>
+      <c r="I7" s="10">
+        <v>1</v>
+      </c>
+      <c r="J7" s="10">
+        <v>224</v>
+      </c>
+      <c r="K7" s="10">
+        <v>5</v>
+      </c>
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
+      <c r="M7" s="10">
+        <v>360</v>
+      </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="12">
+        <f t="shared" si="0"/>
+        <v>497.77777777777777</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="10">
+        <v>5</v>
+      </c>
+      <c r="R7" s="12">
+        <f t="shared" si="1"/>
+        <v>2488.8888888888887</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <f>((25*3.14)/8)</f>
+        <v>9.8125</v>
+      </c>
+      <c r="E8" s="13">
+        <v>800</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="2"/>
+        <v>7850</v>
+      </c>
+      <c r="H8" s="10">
+        <v>38270</v>
+      </c>
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10">
+        <v>1</v>
+      </c>
+      <c r="K8" s="10">
+        <v>1</v>
+      </c>
+      <c r="L8" s="10">
+        <v>1</v>
+      </c>
+      <c r="M8" s="10">
+        <v>360</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="12">
+        <f t="shared" si="0"/>
+        <v>106.30555555555556</v>
+      </c>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="10">
+        <v>10</v>
+      </c>
+      <c r="R8" s="12">
+        <f t="shared" si="1"/>
+        <v>1063.0555555555557</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <f>(1293/64)</f>
+        <v>20.203125</v>
+      </c>
+      <c r="E9" s="13">
+        <v>400</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="2"/>
+        <v>8081.25</v>
+      </c>
+      <c r="H9" s="11">
+        <v>4000</v>
+      </c>
+      <c r="I9" s="11">
+        <v>1</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1293</v>
+      </c>
+      <c r="K9" s="11">
+        <v>64</v>
+      </c>
+      <c r="L9" s="11">
+        <v>1</v>
+      </c>
+      <c r="M9" s="11">
+        <v>360</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="12">
+        <f>(H9/I9)*(J9/K9)*(L9/M9)</f>
+        <v>224.47916666666669</v>
+      </c>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="11">
+        <v>20</v>
+      </c>
+      <c r="R9" s="12">
+        <f>Q9*O9</f>
+        <v>4489.5833333333339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFD2E7A-B27D-4E92-84C9-38B140952E34}">
   <dimension ref="B5:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" customWidth="1"/>
-    <col min="6" max="6" width="15.75" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
-    <col min="8" max="8" width="17.75" customWidth="1"/>
-    <col min="9" max="9" width="3.125" customWidth="1"/>
-    <col min="10" max="10" width="16.625" customWidth="1"/>
-    <col min="11" max="11" width="17.625" customWidth="1"/>
-    <col min="12" max="12" width="23.125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
-    <col min="14" max="14" width="15.25" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:13">
-      <c r="C5" s="7" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="J5" s="7" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="J5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="2:13" ht="43.5" thickBot="1">
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="2:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
@@ -611,7 +1027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="15.75" thickBot="1">
+    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -648,7 +1064,7 @@
         <v>2.2499999999999998E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="15.75" thickBot="1">
+    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -684,7 +1100,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="15.75" thickBot="1">
+    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -720,7 +1136,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="15.75" thickBot="1">
+    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -757,7 +1173,7 @@
         <v>2.0089285714285717E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="15.75" thickBot="1">
+    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -794,7 +1210,7 @@
         <v>9.1719745222929947E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="15.75" thickBot="1">
+    <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -831,7 +1247,7 @@
         <v>4.4547563805104407E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M15" s="2"/>
     </row>
   </sheetData>

</xml_diff>